<commit_message>
Leader and Leader Transitions Set
</commit_message>
<xml_diff>
--- a/MT - Stories.xlsx
+++ b/MT - Stories.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="355">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="356">
   <si>
     <t>Title</t>
   </si>
@@ -97,9 +97,6 @@
     <t>&lt;MTLeader&gt; died</t>
   </si>
   <si>
-    <t>Today is a solemn day.  &lt;MTLeaderTitle&gt; &lt;MTLeader&gt; no longer walks the world of the living.  Martian society would not be what it is today without the indelible touch of &lt;MTLeaderTitle &lt;MTLeader&gt; in so many places.  Please take a moment today to stop by your local spacebar and lift one up in honor of the late, great &lt;MTLeaderTitle&gt;.  What are your best memories of the now former &lt;MTLeaderTitle&gt;?  Send in your letters to the editor.  Select entries will be printed in Thursday’s edition.  Thank you for your service, &lt;MTLeaderTitle&gt;.  You will be missed.</t>
-  </si>
-  <si>
     <t>Mars is in Mourning</t>
   </si>
   <si>
@@ -107,9 +104,6 @@
   </si>
   <si>
     <t>Mars Mourns &lt;MTLeaderTitle&gt;’s Passing</t>
-  </si>
-  <si>
-    <t>&lt;MTLeaderTitle&gt; &lt;MTLeader&gt; served us honorably for many a sol and their passing has not gone unnoticed.  Despite serving Mars well during their tenure, it is suspected that they never quite fully adapted to the realities of life on Mars and between the stresses of daily Martian life, serving as our &lt;MTLeaderTitle&gt;, and many a sleepless night, a heart attack finally took them from us.  May your slumber, &lt;MTLeaderTitle&gt; &lt;MTLeader&gt;, be deep and pleasant.  You will be missed.</t>
   </si>
   <si>
     <t>MTMain.NewLeader.1</t>
@@ -1094,6 +1088,15 @@
   </si>
   <si>
     <t>MTMain.FounderLegacy</t>
+  </si>
+  <si>
+    <t>an idiot colonist</t>
+  </si>
+  <si>
+    <t>Today is a solemn day.  &lt;MTLeaderTitle&gt; &lt;MTDeadLeader&gt; no longer walks the world of the living.  Martian society would not be what it is today without the indelible touch of &lt;MTLeaderTitle &lt;MTDeadLeader&gt; in so many places.  Please take a moment today to stop by your local spacebar and lift one up in honor of the late, great &lt;MTLeaderTitle&gt;.  What are your best memories of the now former &lt;MTLeaderTitle&gt;?  Send in your letters to the editor.  Select entries will be printed in Thursday’s edition.  Thank you for your service, &lt;MTLeaderTitle&gt;.  You will be missed.</t>
+  </si>
+  <si>
+    <t>&lt;MTLeaderTitle&gt; &lt;MTDeadLeader&gt; served us honorably for many a sol and their passing has not gone unnoticed.  Despite serving Mars well during their tenure, it is suspected that they never quite fully adapted to the realities of life on Mars and between the stresses of daily Martian life, serving as our &lt;MTLeaderTitle&gt;, and many a sleepless night, a heart attack finally took them from us.  May your slumber, &lt;MTLeaderTitle&gt; &lt;MTDeadLeader&gt;, be deep and pleasant.  You will be missed.</t>
   </si>
 </sst>
 </file>
@@ -1180,7 +1183,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1233,9 +1236,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
@@ -1246,6 +1246,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1548,30 +1554,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E36"/>
+  <dimension ref="A1:E35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:D13"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22:D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.85546875" style="23" customWidth="1"/>
-    <col min="2" max="2" width="31.28515625" style="23" customWidth="1"/>
-    <col min="3" max="3" width="31.7109375" style="23" customWidth="1"/>
-    <col min="4" max="4" width="112.28515625" style="23" customWidth="1"/>
-    <col min="5" max="5" width="17.5703125" style="23" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="23"/>
+    <col min="1" max="1" width="24.85546875" style="22" customWidth="1"/>
+    <col min="2" max="2" width="31.28515625" style="22" customWidth="1"/>
+    <col min="3" max="3" width="31.7109375" style="22" customWidth="1"/>
+    <col min="4" max="4" width="112.28515625" style="22" customWidth="1"/>
+    <col min="5" max="5" width="17.5703125" style="22" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="22"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="C1" s="22">
+      <c r="B1" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="C1" s="21">
         <v>22</v>
       </c>
     </row>
@@ -1589,18 +1595,18 @@
         <v>1</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="B3" s="14" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>8</v>
@@ -1613,7 +1619,7 @@
     </row>
     <row r="5" spans="1:5" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="B5" s="14" t="s">
         <v>9</v>
@@ -1626,56 +1632,56 @@
       </c>
     </row>
     <row r="7" spans="1:5" s="14" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="19" t="s">
+      <c r="A7" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="19" t="s">
-        <v>73</v>
-      </c>
-      <c r="C7" s="20" t="s">
+      <c r="B7" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="C7" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="19" t="s">
+      <c r="D7" s="24" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="19"/>
-      <c r="B8" s="19"/>
-      <c r="C8" s="20"/>
-      <c r="D8" s="19"/>
+      <c r="A8" s="24"/>
+      <c r="B8" s="24"/>
+      <c r="C8" s="25"/>
+      <c r="D8" s="24"/>
     </row>
     <row r="10" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="C10" s="16" t="s">
+        <v>190</v>
+      </c>
+      <c r="D10" s="17" t="s">
         <v>192</v>
-      </c>
-      <c r="D10" s="17" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="C11" s="16" t="s">
+        <v>191</v>
+      </c>
+      <c r="D11" s="15" t="s">
         <v>193</v>
-      </c>
-      <c r="D11" s="15" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="B13" s="14" t="s">
         <v>15</v>
@@ -1684,226 +1690,226 @@
         <v>16</v>
       </c>
       <c r="D13" s="15" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A15" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15" s="21" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A17" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="D17" s="21" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A19" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="D19" s="19" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B20" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="D20" s="14" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A22" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="B22" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="C22" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="D22" s="14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A23" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="B23" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="C23" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="D23" s="14" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A24" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="B24" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="C24" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="D24" s="14" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" s="14" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="14" t="s">
         <v>343</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A15" s="23" t="s">
-        <v>19</v>
-      </c>
-      <c r="B15" s="23" t="s">
-        <v>18</v>
-      </c>
-      <c r="C15" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="D15" s="22" t="s">
+      <c r="B26" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="C26" s="14" t="s">
         <v>342</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A17" s="23" t="s">
-        <v>22</v>
-      </c>
-      <c r="B17" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="C17" s="24" t="s">
-        <v>21</v>
-      </c>
-      <c r="D17" s="22" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A19" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="B19" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="C19" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="D19" s="22" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A20" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="B20" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="C20" s="23" t="s">
-        <v>29</v>
-      </c>
-      <c r="D20" s="23" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A22" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="B22" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="C22" s="23" t="s">
-        <v>33</v>
-      </c>
-      <c r="D22" s="23" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A23" s="23" t="s">
-        <v>35</v>
-      </c>
-      <c r="B23" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="C23" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="D23" s="23" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A24" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="B24" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="C24" s="24" t="s">
+      <c r="D26" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="D24" s="23" t="s">
+    </row>
+    <row r="27" spans="1:5" s="14" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="14" t="s">
+        <v>346</v>
+      </c>
+      <c r="B27" s="14" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A26" s="23" t="s">
+      <c r="C27" s="14" t="s">
+        <v>140</v>
+      </c>
+      <c r="D27" s="14" t="s">
+        <v>154</v>
+      </c>
+      <c r="E27" s="14" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" s="14" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A28" s="14" t="s">
         <v>345</v>
       </c>
-      <c r="B26" s="23" t="s">
-        <v>42</v>
-      </c>
-      <c r="C26" s="23" t="s">
+      <c r="B28" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="C28" s="14" t="s">
+        <v>153</v>
+      </c>
+      <c r="D28" s="14" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" s="14" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A29" s="14" t="s">
         <v>344</v>
       </c>
-      <c r="D26" s="14" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="23" t="s">
+      <c r="B29" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="C29" s="14" t="s">
+        <v>156</v>
+      </c>
+      <c r="D29" s="14" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" s="14" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A30" s="14" t="s">
+        <v>347</v>
+      </c>
+      <c r="B30" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="C30" s="14" t="s">
+        <v>158</v>
+      </c>
+      <c r="D30" s="14" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" s="14" customFormat="1" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="14" t="s">
         <v>348</v>
       </c>
-      <c r="B27" s="23" t="s">
-        <v>42</v>
-      </c>
-      <c r="C27" s="23" t="s">
-        <v>142</v>
-      </c>
-      <c r="D27" s="14" t="s">
-        <v>156</v>
-      </c>
-      <c r="E27" s="23" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A28" s="23" t="s">
-        <v>347</v>
-      </c>
-      <c r="B28" s="23" t="s">
-        <v>42</v>
-      </c>
-      <c r="C28" s="23" t="s">
-        <v>155</v>
-      </c>
-      <c r="D28" s="14" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A29" s="23" t="s">
-        <v>346</v>
-      </c>
-      <c r="B29" s="23" t="s">
-        <v>42</v>
-      </c>
-      <c r="C29" s="23" t="s">
-        <v>158</v>
-      </c>
-      <c r="D29" s="14" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A30" s="23" t="s">
+      <c r="B31" s="14" t="s">
+        <v>353</v>
+      </c>
+      <c r="C31" s="14" t="s">
+        <v>166</v>
+      </c>
+      <c r="D31" s="17" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D32" s="10"/>
+    </row>
+    <row r="33" spans="1:5" s="14" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="14" t="s">
+        <v>350</v>
+      </c>
+      <c r="B33" s="14" t="s">
         <v>349</v>
       </c>
-      <c r="B30" s="23" t="s">
-        <v>42</v>
-      </c>
-      <c r="C30" s="23" t="s">
+      <c r="C33" s="14" t="s">
         <v>160</v>
       </c>
-      <c r="D30" s="14" t="s">
+      <c r="D33" s="18" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" ht="97.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="23" t="s">
-        <v>350</v>
-      </c>
-      <c r="B31" s="23" t="s">
-        <v>42</v>
-      </c>
-      <c r="C31" s="23" t="s">
-        <v>168</v>
-      </c>
-      <c r="D31" s="10" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" ht="97.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D32" s="10"/>
-    </row>
-    <row r="34" spans="1:5" s="14" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="14" t="s">
-        <v>352</v>
-      </c>
-      <c r="B34" s="14" t="s">
-        <v>351</v>
-      </c>
-      <c r="C34" s="14" t="s">
+      <c r="E33" s="14" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" s="14" customFormat="1" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="14" t="s">
+        <v>163</v>
+      </c>
+      <c r="B35" s="14" t="s">
         <v>162</v>
       </c>
-      <c r="D34" s="18" t="s">
-        <v>163</v>
-      </c>
-      <c r="E34" s="14" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="23" t="s">
+      <c r="C35" s="14" t="s">
+        <v>164</v>
+      </c>
+      <c r="D35" s="17" t="s">
         <v>165</v>
-      </c>
-      <c r="B36" s="23" t="s">
-        <v>164</v>
-      </c>
-      <c r="C36" s="23" t="s">
-        <v>166</v>
-      </c>
-      <c r="D36" s="10" t="s">
-        <v>167</v>
       </c>
     </row>
   </sheetData>
@@ -1940,7 +1946,7 @@
         <v>4</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C1" s="8">
         <v>23</v>
@@ -1960,69 +1966,69 @@
         <v>1</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D3" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="B3" t="s">
-        <v>42</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="E3" t="s">
         <v>83</v>
-      </c>
-      <c r="D3" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="E3" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="81.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C4" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C5" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B8" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C8" t="s">
+        <v>86</v>
+      </c>
+      <c r="D8" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="D8" s="11" t="s">
-        <v>90</v>
-      </c>
       <c r="E8" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -2030,44 +2036,44 @@
     </row>
     <row r="10" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>114</v>
+      </c>
+      <c r="B10" t="s">
+        <v>118</v>
+      </c>
+      <c r="C10" t="s">
+        <v>115</v>
+      </c>
+      <c r="D10" s="10" t="s">
         <v>116</v>
-      </c>
-      <c r="B10" t="s">
-        <v>120</v>
-      </c>
-      <c r="C10" t="s">
-        <v>117</v>
-      </c>
-      <c r="D10" s="10" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>117</v>
+      </c>
+      <c r="B11" t="s">
+        <v>118</v>
+      </c>
+      <c r="C11" t="s">
+        <v>120</v>
+      </c>
+      <c r="D11" s="10" t="s">
         <v>119</v>
-      </c>
-      <c r="B11" t="s">
-        <v>120</v>
-      </c>
-      <c r="C11" t="s">
-        <v>122</v>
-      </c>
-      <c r="D11" s="10" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B12" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="C12" t="s">
         <v>123</v>
       </c>
-      <c r="C12" t="s">
-        <v>125</v>
-      </c>
       <c r="D12" s="10" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -2078,241 +2084,241 @@
     </row>
     <row r="17" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B17" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="C17" t="s">
+        <v>92</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="E17" t="s">
         <v>91</v>
-      </c>
-      <c r="C17" t="s">
-        <v>94</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="E17" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>95</v>
+      </c>
+      <c r="B18" t="s">
+        <v>94</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="D18" s="4" t="s">
         <v>97</v>
-      </c>
-      <c r="B18" t="s">
-        <v>96</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B20" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E20" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C21" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B22" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>110</v>
+      </c>
+      <c r="B23" t="s">
+        <v>111</v>
+      </c>
+      <c r="C23" t="s">
         <v>112</v>
       </c>
-      <c r="B23" t="s">
+      <c r="D23" s="4" t="s">
         <v>113</v>
-      </c>
-      <c r="C23" t="s">
-        <v>114</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>168</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="C24" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="D24" s="10" t="s">
         <v>171</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>172</v>
-      </c>
-      <c r="D24" s="10" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>126</v>
+      </c>
+      <c r="B26" t="s">
+        <v>127</v>
+      </c>
+      <c r="C26" t="s">
         <v>128</v>
       </c>
-      <c r="B26" t="s">
-        <v>129</v>
-      </c>
-      <c r="C26" t="s">
-        <v>130</v>
-      </c>
       <c r="D26" s="10" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E26" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>129</v>
+      </c>
+      <c r="B28" t="s">
+        <v>130</v>
+      </c>
+      <c r="C28" t="s">
         <v>131</v>
       </c>
-      <c r="B28" t="s">
+      <c r="D28" s="4" t="s">
         <v>132</v>
-      </c>
-      <c r="C28" t="s">
-        <v>133</v>
-      </c>
-      <c r="D28" s="4" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B30" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C30" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D30" s="12" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E30" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>146</v>
+      </c>
+      <c r="B32" t="s">
+        <v>147</v>
+      </c>
+      <c r="D32" s="10" t="s">
         <v>148</v>
       </c>
-      <c r="B32" t="s">
-        <v>149</v>
-      </c>
-      <c r="D32" s="10" t="s">
-        <v>150</v>
-      </c>
       <c r="E32" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
+        <v>150</v>
+      </c>
+      <c r="B34" t="s">
+        <v>149</v>
+      </c>
+      <c r="C34" t="s">
         <v>152</v>
       </c>
-      <c r="B34" t="s">
+      <c r="D34" s="10" t="s">
         <v>151</v>
       </c>
-      <c r="C34" t="s">
-        <v>154</v>
-      </c>
-      <c r="D34" s="10" t="s">
-        <v>153</v>
-      </c>
       <c r="E34" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
+        <v>182</v>
+      </c>
+      <c r="B36" t="s">
+        <v>183</v>
+      </c>
+      <c r="C36" t="s">
         <v>184</v>
       </c>
-      <c r="B36" t="s">
+      <c r="D36" s="10" t="s">
         <v>185</v>
-      </c>
-      <c r="C36" t="s">
-        <v>186</v>
-      </c>
-      <c r="D36" s="10" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
+        <v>198</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="D38" s="10" t="s">
         <v>200</v>
-      </c>
-      <c r="B38" s="4" t="s">
-        <v>201</v>
-      </c>
-      <c r="C38" s="4" t="s">
-        <v>199</v>
-      </c>
-      <c r="D38" s="10" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B40" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C40" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D40" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
+        <v>222</v>
+      </c>
+      <c r="B42" t="s">
+        <v>223</v>
+      </c>
+      <c r="C42" t="s">
+        <v>225</v>
+      </c>
+      <c r="D42" s="10" t="s">
         <v>224</v>
-      </c>
-      <c r="B42" t="s">
-        <v>225</v>
-      </c>
-      <c r="C42" t="s">
-        <v>227</v>
-      </c>
-      <c r="D42" s="10" t="s">
-        <v>226</v>
       </c>
     </row>
   </sheetData>
@@ -2343,7 +2349,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C1" s="8">
         <v>22</v>
@@ -2365,285 +2371,285 @@
     </row>
     <row r="3" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>60</v>
+      </c>
+      <c r="B15" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="B15" s="4" t="s">
-        <v>64</v>
-      </c>
       <c r="D15" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B16" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D16" s="4" t="s">
         <v>64</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>65</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D18" s="4" t="s">
         <v>67</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>66</v>
+      </c>
+      <c r="B19" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="D19" s="4" t="s">
         <v>70</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B21" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C21" t="s">
         <v>75</v>
       </c>
-      <c r="C21" t="s">
-        <v>77</v>
-      </c>
       <c r="D21" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B24" t="s">
+        <v>141</v>
+      </c>
+      <c r="C24" t="s">
+        <v>142</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="E24" t="s">
         <v>143</v>
-      </c>
-      <c r="C24" t="s">
-        <v>144</v>
-      </c>
-      <c r="D24" s="10" t="s">
-        <v>146</v>
-      </c>
-      <c r="E24" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>172</v>
+      </c>
+      <c r="B26" t="s">
+        <v>173</v>
+      </c>
+      <c r="C26" t="s">
         <v>174</v>
       </c>
-      <c r="B26" t="s">
+      <c r="D26" s="12" t="s">
         <v>175</v>
-      </c>
-      <c r="C26" t="s">
-        <v>176</v>
-      </c>
-      <c r="D26" s="12" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B28" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C28" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D28" s="10" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B30" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C30" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>217</v>
+      </c>
+      <c r="B31" t="s">
         <v>219</v>
       </c>
-      <c r="B31" t="s">
+      <c r="C31" t="s">
+        <v>220</v>
+      </c>
+      <c r="D31" s="12" t="s">
         <v>221</v>
-      </c>
-      <c r="C31" t="s">
-        <v>222</v>
-      </c>
-      <c r="D31" s="12" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>202</v>
+      </c>
+      <c r="B33" t="s">
+        <v>201</v>
+      </c>
+      <c r="C33" t="s">
         <v>204</v>
       </c>
-      <c r="B33" t="s">
+      <c r="D33" s="10" t="s">
         <v>203</v>
-      </c>
-      <c r="C33" t="s">
-        <v>206</v>
-      </c>
-      <c r="D33" s="10" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
+        <v>206</v>
+      </c>
+      <c r="B34" t="s">
+        <v>207</v>
+      </c>
+      <c r="C34" t="s">
+        <v>205</v>
+      </c>
+      <c r="D34" s="4" t="s">
         <v>208</v>
-      </c>
-      <c r="B34" t="s">
-        <v>209</v>
-      </c>
-      <c r="C34" t="s">
-        <v>207</v>
-      </c>
-      <c r="D34" s="4" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="90.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B37" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C37" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D37" s="10" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B39" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="D39" s="10" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
   </sheetData>
@@ -2667,22 +2673,22 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
@@ -2690,17 +2696,17 @@
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="9" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
@@ -2708,17 +2714,17 @@
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="13" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
@@ -2726,17 +2732,17 @@
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
@@ -2744,17 +2750,17 @@
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="21" spans="1:1" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
@@ -2762,17 +2768,17 @@
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="12" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="25" spans="1:1" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" s="12" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
@@ -2780,17 +2786,17 @@
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="12" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="12" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="29" spans="1:1" ht="45" x14ac:dyDescent="0.25">
       <c r="A29" s="12" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
@@ -2798,17 +2804,17 @@
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="12" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="12" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="33" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="12" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
@@ -2816,17 +2822,17 @@
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="12" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="12" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="37" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="12" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
@@ -2834,17 +2840,17 @@
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" s="12" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" s="12" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="41" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="12" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
@@ -2852,17 +2858,17 @@
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" s="12" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" s="12" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="45" spans="1:1" ht="45" x14ac:dyDescent="0.25">
       <c r="A45" s="12" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
@@ -2870,17 +2876,17 @@
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" s="12" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" s="12" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="49" spans="1:1" ht="45" x14ac:dyDescent="0.25">
       <c r="A49" s="12" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
@@ -2888,17 +2894,17 @@
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" s="12" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" s="12" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="53" spans="1:1" ht="45" x14ac:dyDescent="0.25">
       <c r="A53" s="12" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
@@ -2906,17 +2912,17 @@
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" s="12" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" s="12" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="57" spans="1:1" ht="45" x14ac:dyDescent="0.25">
       <c r="A57" s="12" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
@@ -2924,17 +2930,17 @@
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" s="12" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" s="12" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="61" spans="1:1" ht="45" x14ac:dyDescent="0.25">
       <c r="A61" s="12" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
@@ -2942,17 +2948,17 @@
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" s="12" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" s="12" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="65" spans="1:1" ht="45" x14ac:dyDescent="0.25">
       <c r="A65" s="12" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
@@ -2960,17 +2966,17 @@
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" s="12" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" s="12" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
     </row>
     <row r="69" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A69" s="12" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
@@ -2978,32 +2984,32 @@
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" s="12" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" s="12" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="73" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A73" s="12" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76" s="12" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77" s="12" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="78" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A78" s="12" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.25">
@@ -3011,17 +3017,17 @@
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80" s="12" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81" s="12" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="82" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A82" s="12" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.25">
@@ -3029,12 +3035,12 @@
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A84" s="12" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="85" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A85" s="12" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.25">
@@ -3042,17 +3048,17 @@
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87" s="12" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88" s="12" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="89" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A89" s="12" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.25">
@@ -3060,12 +3066,12 @@
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A91" s="12" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="92" spans="1:1" ht="75" x14ac:dyDescent="0.25">
       <c r="A92" s="12" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.25">
@@ -3073,17 +3079,17 @@
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A94" s="12" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A95" s="12" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="96" spans="1:1" ht="45" x14ac:dyDescent="0.25">
       <c r="A96" s="12" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.25">
@@ -3091,17 +3097,17 @@
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A98" s="12" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A99" s="12" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="100" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A100" s="12" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.25">
@@ -3109,17 +3115,17 @@
     </row>
     <row r="102" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A102" s="12" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A103" s="12" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="104" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A104" s="12" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.25">
@@ -3127,12 +3133,12 @@
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A106" s="12" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
     <row r="107" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A107" s="12" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.25">
@@ -3140,12 +3146,12 @@
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A109" s="12" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="110" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A110" s="12" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.25">
@@ -3153,17 +3159,17 @@
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A112" s="12" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A113" s="12" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="114" spans="1:1" ht="45" x14ac:dyDescent="0.25">
       <c r="A114" s="12" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.25">
@@ -3171,17 +3177,17 @@
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A116" s="12" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A117" s="12" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
     </row>
     <row r="118" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A118" s="12" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.25">
@@ -3189,12 +3195,12 @@
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A120" s="12" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
     </row>
     <row r="121" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A121" s="12" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.25">
@@ -3202,17 +3208,17 @@
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A123" s="12" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A124" s="12" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="125" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A125" s="12" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.25">
@@ -3220,12 +3226,12 @@
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A127" s="12" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="128" spans="1:1" ht="75" x14ac:dyDescent="0.25">
       <c r="A128" s="13" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.25">
@@ -3233,17 +3239,17 @@
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A130" s="12" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A131" s="12" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="132" spans="1:1" ht="45" x14ac:dyDescent="0.25">
       <c r="A132" s="12" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.25">
@@ -3251,17 +3257,17 @@
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A134" s="12" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A135" s="12" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="136" spans="1:1" ht="60" x14ac:dyDescent="0.25">
       <c r="A136" s="12" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.25">
@@ -3269,17 +3275,17 @@
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A138" s="12" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A139" s="12" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
     </row>
     <row r="140" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A140" s="12" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.25">
@@ -3287,12 +3293,12 @@
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A142" s="12" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
     </row>
     <row r="143" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A143" s="12" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.25">
@@ -3300,17 +3306,17 @@
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A145" s="12" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A146" s="12" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
     </row>
     <row r="147" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A147" s="12" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.25">
@@ -3318,17 +3324,17 @@
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A149" s="12" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A150" s="12" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
     </row>
     <row r="151" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A151" s="12" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
vegan1 check and typo correction
</commit_message>
<xml_diff>
--- a/MT - Stories.xlsx
+++ b/MT - Stories.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="90" windowWidth="18195" windowHeight="9795"/>
+    <workbookView xWindow="240" yWindow="90" windowWidth="18195" windowHeight="9795" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="4" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="509" uniqueCount="464">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="508" uniqueCount="464">
   <si>
     <t>Title</t>
   </si>
@@ -1909,7 +1909,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D34" sqref="D34"/>
     </sheetView>
@@ -3613,10 +3613,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A90"/>
+  <dimension ref="A1:A86"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3626,334 +3626,320 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
-        <v>97</v>
-      </c>
+      <c r="A1" s="22"/>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="9"/>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="9"/>
+      <c r="A3" s="9" t="s">
+        <v>447</v>
+      </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>447</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>446</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
         <v>216</v>
       </c>
     </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="9"/>
+    </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" s="9"/>
+      <c r="A8" s="9" t="s">
+        <v>229</v>
+      </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="9" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" s="9"/>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" s="9"/>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" s="9" t="s">
+        <v>232</v>
+      </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A16" s="9" t="s">
         <v>322</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="9" t="s">
+        <v>323</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A20" s="9" t="s">
         <v>325</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="9" t="s">
+        <v>217</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="9" t="s">
         <v>327</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" s="9" t="s">
+        <v>328</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="9" t="s">
         <v>330</v>
       </c>
     </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" s="9"/>
+    </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" s="9"/>
+      <c r="A30" s="9" t="s">
+        <v>335</v>
+      </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="9" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" ht="45" x14ac:dyDescent="0.25">
       <c r="A32" s="9" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A33" s="9" t="s">
         <v>337</v>
       </c>
     </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="9"/>
+    </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" s="9"/>
+      <c r="A34" s="9" t="s">
+        <v>346</v>
+      </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="9" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="9" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A37" s="9" t="s">
         <v>348</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" s="9" t="s">
+        <v>448</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" s="9" t="s">
-        <v>448</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" ht="45" x14ac:dyDescent="0.25">
       <c r="A40" s="9" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A41" s="9" t="s">
         <v>449</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" s="9" t="s">
+        <v>332</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" s="9" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" ht="45" x14ac:dyDescent="0.25">
       <c r="A44" s="9" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A45" s="9" t="s">
         <v>334</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" s="9" t="s">
+        <v>338</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" s="9" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A48" s="9" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" s="9" t="s">
         <v>338</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A48" s="9" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A49" s="9" t="s">
-        <v>340</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" s="9" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" ht="60" x14ac:dyDescent="0.25">
       <c r="A52" s="9" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A53" s="9" t="s">
         <v>342</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" s="9" t="s">
+        <v>343</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" s="9" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" ht="45" x14ac:dyDescent="0.25">
       <c r="A56" s="9" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="57" spans="1:1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A57" s="9" t="s">
         <v>345</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" s="9" t="s">
+        <v>349</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" s="9" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" ht="45" x14ac:dyDescent="0.25">
       <c r="A61" s="9" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="62" spans="1:1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A62" s="9" t="s">
         <v>351</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" s="9" t="s">
+        <v>450</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" s="9" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" ht="60" x14ac:dyDescent="0.25">
       <c r="A65" s="9" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="66" spans="1:1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A66" s="9" t="s">
         <v>353</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A68" s="9"/>
+      <c r="A68" s="9" t="s">
+        <v>358</v>
+      </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A69" s="9"/>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A70" s="9"/>
+      <c r="A69" s="9" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A70" s="9" t="s">
+        <v>360</v>
+      </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" s="9" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" s="9" t="s">
-        <v>359</v>
+        <v>361</v>
       </c>
     </row>
     <row r="74" spans="1:1" ht="45" x14ac:dyDescent="0.25">
       <c r="A74" s="9" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76" s="9" t="s">
-        <v>354</v>
+        <v>444</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77" s="9" t="s">
-        <v>361</v>
+        <v>363</v>
       </c>
     </row>
     <row r="78" spans="1:1" ht="45" x14ac:dyDescent="0.25">
       <c r="A78" s="9" t="s">
-        <v>362</v>
+        <v>364</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80" s="9" t="s">
-        <v>444</v>
+        <v>354</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81" s="9" t="s">
-        <v>363</v>
+        <v>365</v>
       </c>
     </row>
     <row r="82" spans="1:1" ht="45" x14ac:dyDescent="0.25">
       <c r="A82" s="9" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A84" s="9" t="s">
-        <v>354</v>
+      <c r="A84" s="23" t="s">
+        <v>367</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A85" s="9" t="s">
-        <v>365</v>
+      <c r="A85" s="23" t="s">
+        <v>368</v>
       </c>
     </row>
     <row r="86" spans="1:1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A86" s="9" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A88" s="23" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A89" s="23" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="90" spans="1:1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A90" s="23" t="s">
+      <c r="A86" s="23" t="s">
         <v>369</v>
       </c>
     </row>

</xml_diff>